<commit_message>
Add k-means clustering for features.
</commit_message>
<xml_diff>
--- a/Kevin/Knime Workspace/DMC2022_Sandbox/MyOutput/Relative Frequency.xlsx
+++ b/Kevin/Knime Workspace/DMC2022_Sandbox/MyOutput/Relative Frequency.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Number of purchases</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;9</t>
   </si>
 </sst>
 </file>
@@ -68,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -127,13 +131,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -153,15 +165,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C9"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C4:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,6 +264,9 @@
       <c r="C8" s="1" t="n">
         <v>0.00310668643648944</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>106</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -262,6 +278,126 @@
       <c r="C9" s="1" t="n">
         <v>0.00161512391442491</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>298</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="3" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="3" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>